<commit_message>
RWS - removed some bitrot. This stuff shows issue #664
</commit_message>
<xml_diff>
--- a/ZwolleFrontEnd/RWS/Kabeladministratie (fout).xlsx
+++ b/ZwolleFrontEnd/RWS/Kabeladministratie (fout).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
   <si>
     <t>13-69-051</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>+LE60W01-E110.11</t>
-  </si>
-  <si>
-    <t>(is van het soort)</t>
   </si>
   <si>
     <t>=10+TE09R01</t>
@@ -598,7 +595,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,11 +621,11 @@
         <v>14</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G1" s="8"/>
     </row>
@@ -645,15 +642,11 @@
       <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>40</v>
-      </c>
+      <c r="E2" s="8"/>
       <c r="F2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>40</v>
-      </c>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
@@ -804,7 +797,7 @@
         <v>TRANSMISSIEKAST NETWERK</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="4" t="str">
         <f t="shared" si="1"/>
@@ -921,7 +914,7 @@
         <v>Kabel_13-69-061</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="3" t="str">
@@ -966,7 +959,7 @@
         <v>Kabel_13-69-063</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" ref="E15:E22" si="3">IF($D15="","",VLOOKUP($D15,$A$26:$B$39,2,FALSE))</f>
@@ -983,7 +976,7 @@
         <v>Kabel_13-69-064</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1000,7 +993,7 @@
         <v>Kabel_13-69-065</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1017,7 +1010,7 @@
         <v>Kabel_13-69-066</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1034,7 +1027,7 @@
         <v>Kabel_13-69-067</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1051,7 +1044,7 @@
         <v>Kabel_13-69-068</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="3"/>
@@ -1068,7 +1061,7 @@
         <v>Kabel_13-69-069</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>16</v>
@@ -1078,7 +1071,7 @@
         <v/>
       </c>
       <c r="F21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G21" s="4" t="e">
         <f t="shared" si="4"/>
@@ -1091,7 +1084,7 @@
         <v>Kabel_13-69-070</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>16</v>
@@ -1185,7 +1178,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>34</v>

</xml_diff>